<commit_message>
Lots of improvements to overall app
</commit_message>
<xml_diff>
--- a/QuestionResponseFiles/qr_mapping.xlsx
+++ b/QuestionResponseFiles/qr_mapping.xlsx
@@ -42,217 +42,205 @@
     <x:t>Preferred Response</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">C# </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> 10</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">bachelor </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> No</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Bachelor's </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">background check </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Yes</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">phone number </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> 8123455974</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">phone </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Email </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> im10g@hotmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">visa </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">legally authorized to work </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> yes</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">automation </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> 5</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">JavaScript </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">XML </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">onsite </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SQL </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> 8</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Oracle </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Jira </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">hybrid </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Software as a Service </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SaaS </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Java </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Full-Stack </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> 6</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">fullstack </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Web Application </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">commuting </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">AWS </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Amazon Web Services </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">JQUERY </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">HTML </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">.NET </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">react </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">angular </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">first name </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Johnny</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">last name </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Arnett</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">last </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">first </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Google form to be considered </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Google form to be </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">LINKEDIN </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> https://www.linkedin.com/in/johnny-arnett-350959135/</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Secret Clearance </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Clearance </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">secret </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Cover Letter </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Dear Hiring Manager,\n\nWith extensive experience in quality assurance and a proven track record in ensuring software reliability and functionality, I am excited to apply for the {jobtitlerole} role. My expertise in test strategy, automation, and troubleshooting aligns well with your company’s commitment to quality. I am eager to bring my analytical skills and attention to detail to your team.\n\nThank you for considering my application.\n\nSincerely,\nJohnny Arnett</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">drug </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">remote setting </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">desired pay </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> 85000 USD</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">desired salary </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">city </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Evansville</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">address </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> 1000 Western Hills Drive</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">state </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Indiana</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">city* </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">mobile phone number </x:t>
+    <x:t>C#</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>background check</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Yes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>phone number</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8123455974</x:t>
+  </x:si>
+  <x:si>
+    <x:t>phone</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Email</x:t>
+  </x:si>
+  <x:si>
+    <x:t>im10g@hotmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>visa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>No</x:t>
+  </x:si>
+  <x:si>
+    <x:t>legally authorized to work</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>automation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JavaScript</x:t>
+  </x:si>
+  <x:si>
+    <x:t>XML</x:t>
+  </x:si>
+  <x:si>
+    <x:t>onsite</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SQL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Oracle</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jira</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Software as a Service</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SaaS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Java</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-Stack</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>fullstack</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Web Application</x:t>
+  </x:si>
+  <x:si>
+    <x:t>commuting</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AWS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Amazon Web Services</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JQUERY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HTML</x:t>
+  </x:si>
+  <x:si>
+    <x:t>.NET</x:t>
+  </x:si>
+  <x:si>
+    <x:t>react</x:t>
+  </x:si>
+  <x:si>
+    <x:t>angular</x:t>
+  </x:si>
+  <x:si>
+    <x:t>first name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Johnny</x:t>
+  </x:si>
+  <x:si>
+    <x:t>last name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Arnett</x:t>
+  </x:si>
+  <x:si>
+    <x:t>last</x:t>
+  </x:si>
+  <x:si>
+    <x:t>first</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Google form to be considered</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Google form to be</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LINKEDIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.linkedin.com/in/johnny-arnett-350959135/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Secret Clearance</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Clearance</x:t>
+  </x:si>
+  <x:si>
+    <x:t>secret</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cover Letter</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dear Hiring Manager,\n\nWith extensive experience in quality assurance and a proven track record in ensuring software reliability and functionality, I am excited to apply for the {jobtitlerole} role. My expertise in test strategy, automation, and troubleshooting aligns well with your company’s commitment to quality. I am eager to bring my analytical skills and attention to detail to your team.\n\nThank you for considering my application.\n\nSincerely,\nJohnny Arnett</x:t>
+  </x:si>
+  <x:si>
+    <x:t>drug</x:t>
+  </x:si>
+  <x:si>
+    <x:t>remote setting</x:t>
+  </x:si>
+  <x:si>
+    <x:t>desired pay</x:t>
+  </x:si>
+  <x:si>
+    <x:t>85000 USD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>desired salary</x:t>
+  </x:si>
+  <x:si>
+    <x:t>city</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Evansville</x:t>
+  </x:si>
+  <x:si>
+    <x:t>address</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1000 Western Hills Drive</x:t>
+  </x:si>
+  <x:si>
+    <x:t>state</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Indiana</x:t>
+  </x:si>
+  <x:si>
+    <x:t>city*</x:t>
+  </x:si>
+  <x:si>
+    <x:t>mobile phone number</x:t>
   </x:si>
   <x:si>
     <x:t>Disability Status</x:t>
@@ -282,19 +270,55 @@
     <x:t>currently reside in</x:t>
   </x:si>
   <x:si>
-    <x:t>Yes</x:t>
+    <x:t>currently have any family members or relatives working at</x:t>
   </x:si>
   <x:si>
     <x:t>compensation expectations</x:t>
   </x:si>
   <x:si>
-    <x:t>$75,000-90,000</x:t>
-  </x:si>
-  <x:si>
-    <x:t>currently have any family members or relatives working at</x:t>
-  </x:si>
-  <x:si>
-    <x:t>No</x:t>
+    <x:t>75000</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(city*)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>bachelor</x:t>
+  </x:si>
+  <x:si>
+    <x:t>bachelor's</x:t>
+  </x:si>
+  <x:si>
+    <x:t>proficiency in English</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Native or Bilingual</x:t>
+  </x:si>
+  <x:si>
+    <x:t>hybrid setting</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hybrid</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LinkedIn Profile</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ZIP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>47720</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ZIPCODE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ZIP/ Postal Code</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Postal Code</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -680,15 +704,15 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A5" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
         <x:v>7</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -704,28 +728,28 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A8" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A9" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A10" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
         <x:v>16</x:v>
@@ -733,10 +757,10 @@
     </x:row>
     <x:row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A11" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -744,7 +768,7 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -752,47 +776,47 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A14" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A15" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A16" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A17" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
         <x:v>26</x:v>
-      </x:c>
-      <x:c r="B17" s="0" t="s">
-        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A18" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -816,7 +840,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -824,71 +848,71 @@
         <x:v>33</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A23" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A24" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A25" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A26" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A27" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A28" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A29" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A30" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
         <x:v>42</x:v>
-      </x:c>
-      <x:c r="B30" s="0" t="s">
-        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -896,23 +920,23 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A32" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
         <x:v>44</x:v>
-      </x:c>
-      <x:c r="B32" s="0" t="s">
-        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A33" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -920,23 +944,23 @@
         <x:v>47</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A35" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A36" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
         <x:v>50</x:v>
-      </x:c>
-      <x:c r="B36" s="0" t="s">
-        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -944,7 +968,7 @@
         <x:v>51</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -952,7 +976,7 @@
         <x:v>52</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -960,15 +984,15 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A40" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
         <x:v>55</x:v>
-      </x:c>
-      <x:c r="B40" s="0" t="s">
-        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1000,7 +1024,7 @@
         <x:v>60</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1008,39 +1032,39 @@
         <x:v>61</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A46" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A47" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A48" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A49" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1056,39 +1080,39 @@
         <x:v>71</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A52" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:3">
       <x:c r="A53" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:3">
       <x:c r="A54" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:3">
       <x:c r="A55" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:3">
@@ -1104,23 +1128,87 @@
         <x:v>81</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:3">
       <x:c r="A58" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:3">
       <x:c r="A59" s="0" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:3">
+      <x:c r="A60" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="s">
         <x:v>85</x:v>
       </x:c>
-      <x:c r="B59" s="0" t="s">
+    </x:row>
+    <x:row r="61" spans="1:3">
+      <x:c r="A61" s="0" t="s">
         <x:v>86</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:3">
+      <x:c r="A62" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:3">
+      <x:c r="A63" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="B63" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:3">
+      <x:c r="A64" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="B64" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:3">
+      <x:c r="A65" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="B65" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" spans="1:3">
+      <x:c r="A66" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:3">
+      <x:c r="A67" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>91</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>